<commit_message>
Se agrega logica de cálculo de esfuerzos
</commit_message>
<xml_diff>
--- a/data/xlsx/table-q1.xlsx
+++ b/data/xlsx/table-q1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcifuentes\Documents\Proyectos\conveyor-cema-calc\data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{440ADE04-0CC6-4161-9138-F4839BFD5D57}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1118BC8E-19CF-4926-A6D2-7CA994A5B7FA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7380" xr2:uid="{3CB23829-EB1A-4CDD-BB53-0D202BEFA063}"/>
   </bookViews>
@@ -33,81 +33,6 @@
     <t>SCH</t>
   </si>
   <si>
-    <t>2" sch 40</t>
-  </si>
-  <si>
-    <t>2" sch 80</t>
-  </si>
-  <si>
-    <t>2-1/2" sch 40</t>
-  </si>
-  <si>
-    <t>2-1/2" sch 80</t>
-  </si>
-  <si>
-    <t>2-1/2" sch 80****</t>
-  </si>
-  <si>
-    <t>3" sch 40</t>
-  </si>
-  <si>
-    <t>3" sch 80</t>
-  </si>
-  <si>
-    <t>3" 80/10 clad</t>
-  </si>
-  <si>
-    <t>3-1/2" sch 40</t>
-  </si>
-  <si>
-    <t>3-1/2" sch 80</t>
-  </si>
-  <si>
-    <t>3-1/2" 80/10 clad</t>
-  </si>
-  <si>
-    <t>3-1/2" sch 80****</t>
-  </si>
-  <si>
-    <t>4" sch 40</t>
-  </si>
-  <si>
-    <t>4" sch 80</t>
-  </si>
-  <si>
-    <t>4" 80/10 clad</t>
-  </si>
-  <si>
-    <t>4" sch 80****</t>
-  </si>
-  <si>
-    <t>5" sch 40</t>
-  </si>
-  <si>
-    <t>5" sch 80</t>
-  </si>
-  <si>
-    <t>5" 80/10 clad</t>
-  </si>
-  <si>
-    <t>6" sch 40</t>
-  </si>
-  <si>
-    <t>6" sch 80</t>
-  </si>
-  <si>
-    <t>6" 80/10 clad</t>
-  </si>
-  <si>
-    <t>8" sch 40</t>
-  </si>
-  <si>
-    <t>8" sch 80</t>
-  </si>
-  <si>
-    <t>8" 80/10 clad</t>
-  </si>
-  <si>
     <t>SS/CS</t>
   </si>
   <si>
@@ -124,6 +49,81 @@
   </si>
   <si>
     <t>I</t>
+  </si>
+  <si>
+    <t>2  sch 40</t>
+  </si>
+  <si>
+    <t>2  sch 80</t>
+  </si>
+  <si>
+    <t>2-1/2  sch 40</t>
+  </si>
+  <si>
+    <t>2-1/2  sch 80</t>
+  </si>
+  <si>
+    <t>2-1/2  sch 80****</t>
+  </si>
+  <si>
+    <t>3  sch 40</t>
+  </si>
+  <si>
+    <t>3  sch 80</t>
+  </si>
+  <si>
+    <t>3  80/10 clad</t>
+  </si>
+  <si>
+    <t>3-1/2  sch 40</t>
+  </si>
+  <si>
+    <t>3-1/2  sch 80</t>
+  </si>
+  <si>
+    <t>3-1/2  80/10 clad</t>
+  </si>
+  <si>
+    <t>3-1/2  sch 80****</t>
+  </si>
+  <si>
+    <t>4  sch 40</t>
+  </si>
+  <si>
+    <t>4  sch 80</t>
+  </si>
+  <si>
+    <t>4  80/10 clad</t>
+  </si>
+  <si>
+    <t>4  sch 80****</t>
+  </si>
+  <si>
+    <t>5  sch 40</t>
+  </si>
+  <si>
+    <t>5  sch 80</t>
+  </si>
+  <si>
+    <t>5  80/10 clad</t>
+  </si>
+  <si>
+    <t>6  sch 40</t>
+  </si>
+  <si>
+    <t>6  sch 80</t>
+  </si>
+  <si>
+    <t>6  80/10 clad</t>
+  </si>
+  <si>
+    <t>8  sch 40</t>
+  </si>
+  <si>
+    <t>8  sch 80</t>
+  </si>
+  <si>
+    <t>8  80/10 clad</t>
   </si>
 </sst>
 </file>
@@ -635,8 +635,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E2FA420-A9EC-4B78-B045-E1953C786BCD}">
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A2:A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,30 +646,30 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>29</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B2" s="5">
         <v>7288</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="B3" s="9">
         <v>9501</v>
@@ -721,7 +721,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5">
         <v>13832</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B5" s="9">
         <v>17402</v>
@@ -773,7 +773,7 @@
     </row>
     <row r="6" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B6" s="5">
         <v>17402</v>
@@ -799,7 +799,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B7" s="9">
         <v>22413</v>
@@ -825,7 +825,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5">
         <v>28929</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B9" s="9">
         <v>42631</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B10" s="5">
         <v>31120</v>
@@ -903,7 +903,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B11" s="9">
         <v>40821</v>
@@ -929,7 +929,7 @@
     </row>
     <row r="12" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B12" s="5">
         <v>58736</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="13" spans="1:8" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B13" s="9">
         <v>40821</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5">
         <v>41788</v>
@@ -1007,7 +1007,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="B15" s="9">
         <v>55527</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="B16" s="5">
         <v>78223</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="B17" s="9">
         <v>55527</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5">
         <v>70791</v>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B19" s="9">
         <v>96539</v>
@@ -1137,7 +1137,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B20" s="5">
         <v>135502</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="B21" s="9">
         <v>110445</v>
@@ -1189,7 +1189,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="B22" s="5">
         <v>158907</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B23" s="9">
         <v>214041</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="B24" s="5">
         <v>218518</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B25" s="9">
         <v>318681</v>
@@ -1293,7 +1293,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B26" s="13">
         <v>413200</v>

</xml_diff>